<commit_message>
chỉnh sửa một số chi tiết 13:34 25/03/21
</commit_message>
<xml_diff>
--- a/function test.xlsx
+++ b/function test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="129">
   <si>
     <t>stt</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Bấm nút thêm mới</t>
-  </si>
-  <si>
-    <t>Mở form thêm mới</t>
   </si>
   <si>
     <t>Bấm nhân bản thành công</t>
@@ -443,6 +440,27 @@
   </si>
   <si>
     <t>test hiệu năng</t>
+  </si>
+  <si>
+    <t>Mở form thêm mới, data trắng</t>
+  </si>
+  <si>
+    <t>Kết quả thực tế</t>
+  </si>
+  <si>
+    <t>Kết quả mong muốn</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Testcase</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Data Test</t>
   </si>
 </sst>
 </file>
@@ -785,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,27 +816,31 @@
     <col min="3" max="3" width="31.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="30.42578125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="37" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>127</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>128</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -826,7 +848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
@@ -834,7 +856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
@@ -842,302 +864,302 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="2" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="2" t="s">
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="2" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="2" t="s">
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="2" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="2" t="s">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D23" s="2">
+        <v>15</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="D22" s="2">
-        <v>15</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E25" s="2" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>3</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>4</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>56</v>
+      <c r="B29" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1151,7 +1173,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,10 +1208,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1197,113 +1219,113 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1311,7 +1333,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1319,7 +1341,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1367,7 +1389,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1375,88 +1397,88 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1464,7 +1486,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1472,7 +1494,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>